<commit_message>
Some print statement change
</commit_message>
<xml_diff>
--- a/youtubedata.xlsx
+++ b/youtubedata.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -440,12 +436,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>date</t>
+          <t>Title</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Title</t>
+          <t>url</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -453,31 +449,6 @@
           <t>FileType</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>url</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="n">
-        <v>45095.85027147079</v>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Ethra Naal (Sulaikha Manzil Version)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>mp4</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>https://youtube.com/watch?v=8l32-NbQW1E</t>
-        </is>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>